<commit_message>
add admin profile to seed, fix problem in parseSeedData function
</commit_message>
<xml_diff>
--- a/src/seeds/files/005_MalaUva_SeedFile.xlsx
+++ b/src/seeds/files/005_MalaUva_SeedFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nama/Library/CloudStorage/Dropbox/2-NAMA/DEV RSRCS/courses/ROCKTHECODE/CODE/02-deliverables/22_RTC_P13_backend-react/malauva-backend/src/seeds/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1315CFA1-E27D-3E45-B029-B32779855B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15629836-D892-6F4F-8427-71A358FE95EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" activeTab="1" xr2:uid="{52677FAD-7042-B148-9A25-30607DD347FB}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1724" uniqueCount="1177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1724" uniqueCount="1178">
   <si>
     <t>name</t>
   </si>
@@ -6506,19 +6506,22 @@
     <t>U0000</t>
   </si>
   <si>
-    <t>"Admin"</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
-    <t>admin@admin.com</t>
-  </si>
-  <si>
     <t>admin123!@</t>
   </si>
   <si>
-    <t>{"-"}</t>
+    <t>"Admin",</t>
+  </si>
+  <si>
+    <t>"admin",</t>
+  </si>
+  <si>
+    <t>"admin@admin.com",</t>
+  </si>
+  <si>
+    <t>{"-"},</t>
   </si>
 </sst>
 </file>
@@ -9938,7 +9941,7 @@
   <dimension ref="A1:L194"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10001,22 +10004,22 @@
         <v>1171</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>1176</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>1173</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>1177</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>1172</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1173</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>1174</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>1175</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>1176</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>1173</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10050,7 +10053,7 @@
       </c>
       <c r="L3" s="1">
         <f ca="1">RANDBETWEEN(1,100) + 1000</f>
-        <v>1027</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10077,14 +10080,14 @@
       </c>
       <c r="I4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4058000</v>
+        <v>4266000</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" ref="L4:L67" ca="1" si="1">RANDBETWEEN(1,100) + 1000</f>
-        <v>1057</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10111,14 +10114,14 @@
       </c>
       <c r="I5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4052197</v>
+        <v>4089304</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1079</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10145,14 +10148,14 @@
       </c>
       <c r="I6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4198877</v>
+        <v>4085937</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1036</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10179,14 +10182,14 @@
       </c>
       <c r="I7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4216375</v>
+        <v>4601368</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1014</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10213,14 +10216,14 @@
       </c>
       <c r="I8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4324625</v>
+        <v>4407911</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1075</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10247,14 +10250,14 @@
       </c>
       <c r="I9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4207464</v>
+        <v>4109319</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1091</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10281,14 +10284,14 @@
       </c>
       <c r="I10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4828688</v>
+        <v>4060648</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1088</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10315,14 +10318,14 @@
       </c>
       <c r="I11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4524552</v>
+        <v>4059261</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L11" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1013</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10349,14 +10352,14 @@
       </c>
       <c r="I12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4828688</v>
+        <v>4109319</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L12" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1092</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10383,14 +10386,14 @@
       </c>
       <c r="I13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4991192</v>
+        <v>4276981</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L13" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1071</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10417,14 +10420,14 @@
       </c>
       <c r="I14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4175000</v>
+        <v>4109319</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10451,14 +10454,14 @@
       </c>
       <c r="I15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4934736</v>
+        <v>4050008</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L15" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1042</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10485,14 +10488,14 @@
       </c>
       <c r="I16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4266000</v>
+        <v>4054096</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L16" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1052</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10519,14 +10522,14 @@
       </c>
       <c r="I17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4071952</v>
+        <v>4364432</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1036</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10553,14 +10556,14 @@
       </c>
       <c r="I18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4059261</v>
+        <v>4051331</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1024</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10587,14 +10590,14 @@
       </c>
       <c r="I19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4378509</v>
+        <v>4141125</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L19" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1047</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10621,14 +10624,14 @@
       </c>
       <c r="I20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4207464</v>
+        <v>4069683</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L20" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1043</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10655,14 +10658,14 @@
       </c>
       <c r="I21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4350763</v>
+        <v>4423248</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L21" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1022</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10689,14 +10692,14 @@
       </c>
       <c r="I22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4471875</v>
+        <v>4190608</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L22" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1061</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10723,14 +10726,14 @@
       </c>
       <c r="I23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4393000</v>
+        <v>4141125</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L23" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1027</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10757,14 +10760,14 @@
       </c>
       <c r="I24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4050008</v>
+        <v>4245112</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L24" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1015</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10791,14 +10794,14 @@
       </c>
       <c r="I25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4245112</v>
+        <v>4129507</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L25" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1027</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10825,14 +10828,14 @@
       </c>
       <c r="I26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4071952</v>
+        <v>4601368</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L26" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1065</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10859,14 +10862,14 @@
       </c>
       <c r="I27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4300047</v>
+        <v>4052744</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L27" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1089</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10893,14 +10896,14 @@
       </c>
       <c r="I28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>5050000</v>
+        <v>4803571</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L28" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1079</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10927,14 +10930,14 @@
       </c>
       <c r="I29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4054096</v>
+        <v>4056859</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L29" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1046</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10961,14 +10964,14 @@
       </c>
       <c r="I30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4364432</v>
+        <v>4378509</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L30" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1021</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -10995,14 +10998,14 @@
       </c>
       <c r="I31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>5050000</v>
+        <v>4104872</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1047</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11029,14 +11032,14 @@
       </c>
       <c r="I32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4050125</v>
+        <v>4056859</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L32" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1010</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11063,14 +11066,14 @@
       </c>
       <c r="I33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4407911</v>
+        <v>4506533</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L33" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1006</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11097,14 +11100,14 @@
       </c>
       <c r="I34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4664125</v>
+        <v>4129507</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L34" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1059</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11131,14 +11134,14 @@
       </c>
       <c r="I35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4050008</v>
+        <v>4054913</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L35" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1061</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11165,14 +11168,14 @@
       </c>
       <c r="I36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4524552</v>
+        <v>4050008</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L36" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1094</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11199,14 +11202,14 @@
       </c>
       <c r="I37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4378509</v>
+        <v>4054096</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L37" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1094</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11233,14 +11236,14 @@
       </c>
       <c r="I38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4300047</v>
+        <v>4471875</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L38" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1079</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11267,14 +11270,14 @@
       </c>
       <c r="I39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4160592</v>
+        <v>4506533</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L39" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1057</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11301,14 +11304,14 @@
       </c>
       <c r="I40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4407911</v>
+        <v>4153823</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L40" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1001</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11335,14 +11338,14 @@
       </c>
       <c r="I41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4109319</v>
+        <v>4052197</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L41" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1069</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11369,14 +11372,14 @@
       </c>
       <c r="I42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4350763</v>
+        <v>4207464</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L42" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1022</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11403,14 +11406,14 @@
       </c>
       <c r="I43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4050064</v>
+        <v>4731472</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L43" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1038</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11437,14 +11440,14 @@
       </c>
       <c r="I44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4312144</v>
+        <v>4109319</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L44" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1018</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11471,14 +11474,14 @@
       </c>
       <c r="I45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4051728</v>
+        <v>4488976</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L45" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1027</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11505,14 +11508,14 @@
       </c>
       <c r="I46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4147336</v>
+        <v>4050125</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L46" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1031</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11539,14 +11542,14 @@
       </c>
       <c r="I47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4153823</v>
+        <v>4225616</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L47" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1065</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11573,14 +11576,14 @@
       </c>
       <c r="I48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4543039</v>
+        <v>4198877</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L48" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1029</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11607,14 +11610,14 @@
       </c>
       <c r="I49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4051000</v>
+        <v>4089304</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L49" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1056</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11641,14 +11644,14 @@
       </c>
       <c r="I50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4471875</v>
+        <v>4524552</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L50" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1060</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11675,14 +11678,14 @@
       </c>
       <c r="I51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4423248</v>
+        <v>4054913</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L51" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1060</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11709,14 +11712,14 @@
       </c>
       <c r="I52" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4069683</v>
+        <v>4378509</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L52" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1067</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11743,14 +11746,14 @@
       </c>
       <c r="I53" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4050027</v>
+        <v>4455224</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L53" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1040</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11777,14 +11780,14 @@
       </c>
       <c r="I54" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4050001</v>
+        <v>4100653</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L54" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1029</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11811,14 +11814,14 @@
       </c>
       <c r="I55" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4118921</v>
+        <v>4167649</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L55" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1077</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11845,14 +11848,14 @@
       </c>
       <c r="I56" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4664125</v>
+        <v>4288328</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L56" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1086</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11879,14 +11882,14 @@
       </c>
       <c r="I57" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4506533</v>
+        <v>4182651</v>
       </c>
       <c r="J57" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L57" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1089</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11913,14 +11916,14 @@
       </c>
       <c r="I58" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4050001</v>
+        <v>4058000</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L58" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1003</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11947,14 +11950,14 @@
       </c>
       <c r="I59" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4153823</v>
+        <v>4779000</v>
       </c>
       <c r="J59" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L59" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1040</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -11981,14 +11984,14 @@
       </c>
       <c r="I60" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4054913</v>
+        <v>4063824</v>
       </c>
       <c r="J60" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L60" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1002</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12015,14 +12018,14 @@
       </c>
       <c r="I61" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4085937</v>
+        <v>4089304</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L61" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1071</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12049,14 +12052,14 @@
       </c>
       <c r="I62" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4506533</v>
+        <v>4050216</v>
       </c>
       <c r="J62" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L62" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1092</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="63" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12083,14 +12086,14 @@
       </c>
       <c r="I63" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4135184</v>
+        <v>4288328</v>
       </c>
       <c r="J63" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L63" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1048</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12117,7 +12120,7 @@
       </c>
       <c r="I64" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4118921</v>
+        <v>4054913</v>
       </c>
       <c r="J64" s="1" t="s">
         <v>14</v>
@@ -12151,14 +12154,14 @@
       </c>
       <c r="I65" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4934736</v>
+        <v>4153823</v>
       </c>
       <c r="J65" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L65" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1047</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="66" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12185,14 +12188,14 @@
       </c>
       <c r="I66" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4754969</v>
+        <v>4058000</v>
       </c>
       <c r="J66" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L66" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1086</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="67" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12219,14 +12222,14 @@
       </c>
       <c r="I67" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4124088</v>
+        <v>4050512</v>
       </c>
       <c r="J67" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L67" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1082</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="68" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12253,14 +12256,14 @@
       </c>
       <c r="I68" s="1">
         <f t="shared" ref="I68:I112" ca="1" si="2">RANDBETWEEN(1,100) ^ 3 + 4050000</f>
-        <v>4524552</v>
+        <v>4350763</v>
       </c>
       <c r="J68" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L68" s="1">
         <f t="shared" ref="L68:L112" ca="1" si="3">RANDBETWEEN(1,100) + 1000</f>
-        <v>1049</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12287,14 +12290,14 @@
       </c>
       <c r="I69" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4245112</v>
+        <v>4364432</v>
       </c>
       <c r="J69" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L69" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1100</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="70" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12321,14 +12324,14 @@
       </c>
       <c r="I70" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4207464</v>
+        <v>4050027</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L70" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1067</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12355,14 +12358,14 @@
       </c>
       <c r="I71" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4601368</v>
+        <v>4050125</v>
       </c>
       <c r="J71" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L71" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1009</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12389,14 +12392,14 @@
       </c>
       <c r="I72" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4050001</v>
+        <v>4053375</v>
       </c>
       <c r="J72" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L72" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1063</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="73" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12423,14 +12426,14 @@
       </c>
       <c r="I73" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>5050000</v>
+        <v>4207464</v>
       </c>
       <c r="J73" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L73" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1062</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="74" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12457,14 +12460,14 @@
       </c>
       <c r="I74" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4423248</v>
+        <v>4324625</v>
       </c>
       <c r="J74" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L74" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1088</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="75" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12491,14 +12494,14 @@
       </c>
       <c r="I75" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4050027</v>
+        <v>4077000</v>
       </c>
       <c r="J75" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L75" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1069</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="76" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12525,14 +12528,14 @@
       </c>
       <c r="I76" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4109319</v>
+        <v>4312144</v>
       </c>
       <c r="J76" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L76" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1082</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="77" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12559,14 +12562,14 @@
       </c>
       <c r="I77" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4991192</v>
+        <v>4096656</v>
       </c>
       <c r="J77" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L77" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1054</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="78" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12593,14 +12596,14 @@
       </c>
       <c r="I78" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4063824</v>
+        <v>4050512</v>
       </c>
       <c r="J78" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L78" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1080</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="79" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12627,14 +12630,14 @@
       </c>
       <c r="I79" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4067576</v>
+        <v>4488976</v>
       </c>
       <c r="J79" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L79" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1081</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="80" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12661,14 +12664,14 @@
       </c>
       <c r="I80" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4803571</v>
+        <v>4124088</v>
       </c>
       <c r="J80" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L80" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1016</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="81" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12695,14 +12698,14 @@
       </c>
       <c r="I81" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4058000</v>
+        <v>4337496</v>
       </c>
       <c r="J81" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L81" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1022</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="82" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12729,14 +12732,14 @@
       </c>
       <c r="I82" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4050001</v>
+        <v>4069683</v>
       </c>
       <c r="J82" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L82" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1033</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="83" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12763,14 +12766,14 @@
       </c>
       <c r="I83" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4488976</v>
+        <v>4077000</v>
       </c>
       <c r="J83" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L83" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1087</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="84" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12797,14 +12800,14 @@
       </c>
       <c r="I84" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4147336</v>
+        <v>4050343</v>
       </c>
       <c r="J84" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L84" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1002</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="85" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12831,14 +12834,14 @@
       </c>
       <c r="I85" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4581441</v>
+        <v>4050008</v>
       </c>
       <c r="J85" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L85" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1091</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="86" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12865,14 +12868,14 @@
       </c>
       <c r="I86" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4062167</v>
+        <v>4266000</v>
       </c>
       <c r="J86" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L86" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1091</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="87" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12899,14 +12902,14 @@
       </c>
       <c r="I87" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4198877</v>
+        <v>4288328</v>
       </c>
       <c r="J87" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L87" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1100</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="88" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12933,14 +12936,14 @@
       </c>
       <c r="I88" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4079791</v>
+        <v>4118921</v>
       </c>
       <c r="J88" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L88" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1081</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="89" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -12967,14 +12970,14 @@
       </c>
       <c r="I89" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4562000</v>
+        <v>4266000</v>
       </c>
       <c r="J89" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L89" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1004</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="90" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -13001,14 +13004,14 @@
       </c>
       <c r="I90" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4288328</v>
+        <v>4664125</v>
       </c>
       <c r="J90" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L90" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1073</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="91" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -13035,14 +13038,14 @@
       </c>
       <c r="I91" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4754969</v>
+        <v>4182651</v>
       </c>
       <c r="J91" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L91" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1068</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="92" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -13069,14 +13072,14 @@
       </c>
       <c r="I92" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4754969</v>
+        <v>4378509</v>
       </c>
       <c r="J92" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L92" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1040</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="93" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -13103,14 +13106,14 @@
       </c>
       <c r="I93" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4642704</v>
+        <v>4828688</v>
       </c>
       <c r="J93" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L93" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="94" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -13137,14 +13140,14 @@
       </c>
       <c r="I94" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4190608</v>
+        <v>4175000</v>
       </c>
       <c r="J94" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L94" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1044</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="95" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -13171,14 +13174,14 @@
       </c>
       <c r="I95" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4225616</v>
+        <v>4050008</v>
       </c>
       <c r="J95" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L95" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1093</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="96" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -13205,14 +13208,14 @@
       </c>
       <c r="I96" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4754969</v>
+        <v>4543039</v>
       </c>
       <c r="J96" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L96" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1078</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="97" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -13239,14 +13242,14 @@
       </c>
       <c r="I97" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4455224</v>
+        <v>4601368</v>
       </c>
       <c r="J97" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L97" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1029</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="98" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -13273,14 +13276,14 @@
       </c>
       <c r="I98" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4147336</v>
+        <v>4109319</v>
       </c>
       <c r="J98" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L98" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1003</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="99" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -13307,14 +13310,14 @@
       </c>
       <c r="I99" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4562000</v>
+        <v>4601368</v>
       </c>
       <c r="J99" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L99" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1012</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="100" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -13341,14 +13344,14 @@
       </c>
       <c r="I100" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4524552</v>
+        <v>4092875</v>
       </c>
       <c r="J100" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L100" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1022</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="101" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -13375,14 +13378,14 @@
       </c>
       <c r="I101" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4350763</v>
+        <v>4050216</v>
       </c>
       <c r="J101" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L101" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1010</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -13409,14 +13412,14 @@
       </c>
       <c r="I102" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4962673</v>
+        <v>4198877</v>
       </c>
       <c r="J102" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L102" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1049</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="103" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -13443,7 +13446,7 @@
       </c>
       <c r="I103" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4050125</v>
+        <v>4077000</v>
       </c>
       <c r="J103" s="1" t="s">
         <v>14</v>
@@ -13477,14 +13480,14 @@
       </c>
       <c r="I104" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4050729</v>
+        <v>4378509</v>
       </c>
       <c r="J104" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L104" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1082</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="105" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -13511,14 +13514,14 @@
       </c>
       <c r="I105" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4053375</v>
+        <v>4059261</v>
       </c>
       <c r="J105" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L105" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1024</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="106" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -13545,14 +13548,14 @@
       </c>
       <c r="I106" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4050008</v>
+        <v>4074389</v>
       </c>
       <c r="J106" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L106" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1044</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="107" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -13579,14 +13582,14 @@
       </c>
       <c r="I107" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4051000</v>
+        <v>4063824</v>
       </c>
       <c r="J107" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L107" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1002</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="108" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -13613,14 +13616,14 @@
       </c>
       <c r="I108" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4153823</v>
+        <v>4907375</v>
       </c>
       <c r="J108" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L108" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="109" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -13647,14 +13650,14 @@
       </c>
       <c r="I109" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4050027</v>
+        <v>4074389</v>
       </c>
       <c r="J109" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L109" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1059</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="110" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -13681,14 +13684,14 @@
       </c>
       <c r="I110" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4054913</v>
+        <v>4079791</v>
       </c>
       <c r="J110" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L110" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1073</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="111" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -13715,14 +13718,14 @@
       </c>
       <c r="I111" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>5020299</v>
+        <v>4062167</v>
       </c>
       <c r="J111" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L111" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1092</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="112" spans="1:12" ht="17" x14ac:dyDescent="0.25">
@@ -13746,14 +13749,14 @@
       </c>
       <c r="I112" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4050216</v>
+        <v>4055832</v>
       </c>
       <c r="J112" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L112" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1006</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="113" spans="2:5" ht="17" x14ac:dyDescent="0.25">
@@ -14175,7 +14178,7 @@
     <hyperlink ref="E50:E86" r:id="rId4" display="passwordTest123!@" xr:uid="{6B123D3C-2392-EB4D-BF68-1342EB39B495}"/>
     <hyperlink ref="E87" r:id="rId5" xr:uid="{DA4BB4F4-75EF-6C48-A8CE-38853F2C61D7}"/>
     <hyperlink ref="E88:E112" r:id="rId6" display="passwordTest123!@" xr:uid="{52F2F631-0F30-D645-A36D-20BF2B3002D4}"/>
-    <hyperlink ref="D2" r:id="rId7" xr:uid="{2B5714BE-5C05-E14B-AE60-A7F40BC2F47C}"/>
+    <hyperlink ref="D2" r:id="rId7" display="admin@admin.com" xr:uid="{2B5714BE-5C05-E14B-AE60-A7F40BC2F47C}"/>
     <hyperlink ref="E2" r:id="rId8" xr:uid="{3102DA88-D705-084A-9896-FE9BD69304B1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14233,7 +14236,7 @@
       </c>
       <c r="B2" s="1">
         <f ca="1">RANDBETWEEN(1,100) + 3000</f>
-        <v>3086</v>
+        <v>3038</v>
       </c>
       <c r="C2" s="1">
         <v>1001</v>
@@ -14251,7 +14254,7 @@
       </c>
       <c r="B3" s="1">
         <f t="shared" ref="B3:B66" ca="1" si="0">RANDBETWEEN(1,100) + 3000</f>
-        <v>3080</v>
+        <v>3003</v>
       </c>
       <c r="C3" s="1">
         <v>1002</v>
@@ -14269,7 +14272,7 @@
       </c>
       <c r="B4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3071</v>
+        <v>3009</v>
       </c>
       <c r="C4" s="1">
         <v>1003</v>
@@ -14287,7 +14290,7 @@
       </c>
       <c r="B5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3063</v>
+        <v>3049</v>
       </c>
       <c r="C5" s="1">
         <v>1004</v>
@@ -14305,7 +14308,7 @@
       </c>
       <c r="B6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3032</v>
+        <v>3056</v>
       </c>
       <c r="C6" s="1">
         <v>1005</v>
@@ -14323,7 +14326,7 @@
       </c>
       <c r="B7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3036</v>
+        <v>3095</v>
       </c>
       <c r="C7" s="1">
         <v>1006</v>
@@ -14341,7 +14344,7 @@
       </c>
       <c r="B8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3092</v>
+        <v>3044</v>
       </c>
       <c r="C8" s="1">
         <v>1007</v>
@@ -14359,7 +14362,7 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3077</v>
+        <v>3027</v>
       </c>
       <c r="C9" s="1">
         <v>1008</v>
@@ -14377,7 +14380,7 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3007</v>
+        <v>3080</v>
       </c>
       <c r="C10" s="1">
         <v>1009</v>
@@ -14395,7 +14398,7 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3074</v>
+        <v>3070</v>
       </c>
       <c r="C11" s="1">
         <v>1010</v>
@@ -14413,7 +14416,7 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3013</v>
+        <v>3028</v>
       </c>
       <c r="C12" s="1">
         <v>1011</v>
@@ -14431,7 +14434,7 @@
       </c>
       <c r="B13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3077</v>
+        <v>3028</v>
       </c>
       <c r="C13" s="1">
         <v>1012</v>
@@ -14449,7 +14452,7 @@
       </c>
       <c r="B14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3029</v>
+        <v>3020</v>
       </c>
       <c r="C14" s="1">
         <v>1013</v>
@@ -14467,7 +14470,7 @@
       </c>
       <c r="B15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3020</v>
+        <v>3061</v>
       </c>
       <c r="C15" s="1">
         <v>1014</v>
@@ -14485,7 +14488,7 @@
       </c>
       <c r="B16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3086</v>
+        <v>3076</v>
       </c>
       <c r="C16" s="1">
         <v>1015</v>
@@ -14503,7 +14506,7 @@
       </c>
       <c r="B17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3061</v>
+        <v>3053</v>
       </c>
       <c r="C17" s="1">
         <v>1016</v>
@@ -14521,7 +14524,7 @@
       </c>
       <c r="B18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3053</v>
+        <v>3055</v>
       </c>
       <c r="C18" s="1">
         <v>1017</v>
@@ -14539,7 +14542,7 @@
       </c>
       <c r="B19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3073</v>
+        <v>3100</v>
       </c>
       <c r="C19" s="1">
         <v>1018</v>
@@ -14557,7 +14560,7 @@
       </c>
       <c r="B20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3033</v>
+        <v>3094</v>
       </c>
       <c r="C20" s="1">
         <v>1019</v>
@@ -14575,7 +14578,7 @@
       </c>
       <c r="B21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3053</v>
+        <v>3048</v>
       </c>
       <c r="C21" s="1">
         <v>1020</v>
@@ -14593,7 +14596,7 @@
       </c>
       <c r="B22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3009</v>
+        <v>3052</v>
       </c>
       <c r="C22" s="1">
         <v>1021</v>
@@ -14611,7 +14614,7 @@
       </c>
       <c r="B23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3002</v>
+        <v>3053</v>
       </c>
       <c r="C23" s="1">
         <v>1022</v>
@@ -14629,7 +14632,7 @@
       </c>
       <c r="B24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3091</v>
+        <v>3097</v>
       </c>
       <c r="C24" s="1">
         <v>1023</v>
@@ -14647,7 +14650,7 @@
       </c>
       <c r="B25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3086</v>
+        <v>3069</v>
       </c>
       <c r="C25" s="1">
         <v>1024</v>
@@ -14665,7 +14668,7 @@
       </c>
       <c r="B26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3068</v>
+        <v>3084</v>
       </c>
       <c r="C26" s="1">
         <v>1025</v>
@@ -14683,7 +14686,7 @@
       </c>
       <c r="B27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3090</v>
+        <v>3034</v>
       </c>
       <c r="C27" s="1">
         <v>1026</v>
@@ -14701,7 +14704,7 @@
       </c>
       <c r="B28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3035</v>
+        <v>3086</v>
       </c>
       <c r="C28" s="1">
         <v>1027</v>
@@ -14719,7 +14722,7 @@
       </c>
       <c r="B29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3030</v>
+        <v>3027</v>
       </c>
       <c r="C29" s="1">
         <v>1028</v>
@@ -14737,7 +14740,7 @@
       </c>
       <c r="B30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3100</v>
+        <v>3079</v>
       </c>
       <c r="C30" s="1">
         <v>1029</v>
@@ -14755,7 +14758,7 @@
       </c>
       <c r="B31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3072</v>
+        <v>3021</v>
       </c>
       <c r="C31" s="1">
         <v>1030</v>
@@ -14773,7 +14776,7 @@
       </c>
       <c r="B32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3065</v>
+        <v>3055</v>
       </c>
       <c r="C32" s="1">
         <v>1031</v>
@@ -14791,7 +14794,7 @@
       </c>
       <c r="B33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3029</v>
+        <v>3084</v>
       </c>
       <c r="C33" s="1">
         <v>1032</v>
@@ -14809,7 +14812,7 @@
       </c>
       <c r="B34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3018</v>
+        <v>3096</v>
       </c>
       <c r="C34" s="1">
         <v>1033</v>
@@ -14827,7 +14830,7 @@
       </c>
       <c r="B35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3070</v>
+        <v>3039</v>
       </c>
       <c r="C35" s="1">
         <v>1034</v>
@@ -14845,7 +14848,7 @@
       </c>
       <c r="B36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3064</v>
+        <v>3061</v>
       </c>
       <c r="C36" s="1">
         <v>1035</v>
@@ -14863,7 +14866,7 @@
       </c>
       <c r="B37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3031</v>
+        <v>3079</v>
       </c>
       <c r="C37" s="1">
         <v>1036</v>
@@ -14881,7 +14884,7 @@
       </c>
       <c r="B38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3012</v>
+        <v>3015</v>
       </c>
       <c r="C38" s="1">
         <v>1037</v>
@@ -14899,7 +14902,7 @@
       </c>
       <c r="B39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3015</v>
+        <v>3019</v>
       </c>
       <c r="C39" s="1">
         <v>1038</v>
@@ -14917,7 +14920,7 @@
       </c>
       <c r="B40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3048</v>
+        <v>3050</v>
       </c>
       <c r="C40" s="1">
         <v>1039</v>
@@ -14935,7 +14938,7 @@
       </c>
       <c r="B41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3096</v>
+        <v>3089</v>
       </c>
       <c r="C41" s="1">
         <v>1040</v>
@@ -14953,7 +14956,7 @@
       </c>
       <c r="B42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3063</v>
+        <v>3005</v>
       </c>
       <c r="C42" s="1">
         <v>1041</v>
@@ -14971,7 +14974,7 @@
       </c>
       <c r="B43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3040</v>
+        <v>3058</v>
       </c>
       <c r="C43" s="1">
         <v>1042</v>
@@ -14989,7 +14992,7 @@
       </c>
       <c r="B44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3018</v>
+        <v>3003</v>
       </c>
       <c r="C44" s="1">
         <v>1043</v>
@@ -15007,7 +15010,7 @@
       </c>
       <c r="B45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3043</v>
+        <v>3015</v>
       </c>
       <c r="C45" s="1">
         <v>1044</v>
@@ -15025,7 +15028,7 @@
       </c>
       <c r="B46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3085</v>
+        <v>3088</v>
       </c>
       <c r="C46" s="1">
         <v>1045</v>
@@ -15043,7 +15046,7 @@
       </c>
       <c r="B47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3029</v>
+        <v>3061</v>
       </c>
       <c r="C47" s="1">
         <v>1046</v>
@@ -15061,7 +15064,7 @@
       </c>
       <c r="B48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3018</v>
+        <v>3010</v>
       </c>
       <c r="C48" s="1">
         <v>1047</v>
@@ -15079,7 +15082,7 @@
       </c>
       <c r="B49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3073</v>
+        <v>3016</v>
       </c>
       <c r="C49" s="1">
         <v>1048</v>
@@ -15097,7 +15100,7 @@
       </c>
       <c r="B50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3042</v>
+        <v>3089</v>
       </c>
       <c r="C50" s="1">
         <v>1049</v>
@@ -15115,7 +15118,7 @@
       </c>
       <c r="B51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3033</v>
+        <v>3038</v>
       </c>
       <c r="C51" s="1">
         <v>1050</v>
@@ -15133,7 +15136,7 @@
       </c>
       <c r="B52" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3038</v>
+        <v>3077</v>
       </c>
       <c r="C52" s="1">
         <v>1051</v>
@@ -15151,7 +15154,7 @@
       </c>
       <c r="B53" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3010</v>
+        <v>3002</v>
       </c>
       <c r="C53" s="1">
         <v>1052</v>
@@ -15169,7 +15172,7 @@
       </c>
       <c r="B54" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3047</v>
+        <v>3004</v>
       </c>
       <c r="C54" s="1">
         <v>1053</v>
@@ -15187,7 +15190,7 @@
       </c>
       <c r="B55" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3049</v>
+        <v>3041</v>
       </c>
       <c r="C55" s="1">
         <v>1054</v>
@@ -15205,7 +15208,7 @@
       </c>
       <c r="B56" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3063</v>
+        <v>3048</v>
       </c>
       <c r="C56" s="1">
         <v>1055</v>
@@ -15223,7 +15226,7 @@
       </c>
       <c r="B57" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3061</v>
+        <v>3094</v>
       </c>
       <c r="C57" s="1">
         <v>1056</v>
@@ -15241,7 +15244,7 @@
       </c>
       <c r="B58" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3077</v>
+        <v>3052</v>
       </c>
       <c r="C58" s="1">
         <v>1057</v>
@@ -15259,7 +15262,7 @@
       </c>
       <c r="B59" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3010</v>
+        <v>3002</v>
       </c>
       <c r="C59" s="1">
         <v>1058</v>
@@ -15277,7 +15280,7 @@
       </c>
       <c r="B60" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3075</v>
+        <v>3013</v>
       </c>
       <c r="C60" s="1">
         <v>1059</v>
@@ -15295,7 +15298,7 @@
       </c>
       <c r="B61" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3012</v>
+        <v>3025</v>
       </c>
       <c r="C61" s="1">
         <v>1060</v>
@@ -15313,7 +15316,7 @@
       </c>
       <c r="B62" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3037</v>
+        <v>3053</v>
       </c>
       <c r="C62" s="1">
         <v>1061</v>
@@ -15331,7 +15334,7 @@
       </c>
       <c r="B63" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3067</v>
+        <v>3076</v>
       </c>
       <c r="C63" s="1">
         <v>1062</v>
@@ -15349,7 +15352,7 @@
       </c>
       <c r="B64" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3013</v>
+        <v>3072</v>
       </c>
       <c r="C64" s="1">
         <v>1063</v>
@@ -15367,7 +15370,7 @@
       </c>
       <c r="B65" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3027</v>
+        <v>3032</v>
       </c>
       <c r="C65" s="1">
         <v>1064</v>
@@ -15385,7 +15388,7 @@
       </c>
       <c r="B66" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3059</v>
+        <v>3063</v>
       </c>
       <c r="C66" s="1">
         <v>1065</v>
@@ -15403,7 +15406,7 @@
       </c>
       <c r="B67" s="1">
         <f t="shared" ref="B67:B110" ca="1" si="1">RANDBETWEEN(1,100) + 3000</f>
-        <v>3004</v>
+        <v>3082</v>
       </c>
       <c r="C67" s="1">
         <v>1066</v>
@@ -15421,7 +15424,7 @@
       </c>
       <c r="B68" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3061</v>
+        <v>3088</v>
       </c>
       <c r="C68" s="1">
         <v>1067</v>
@@ -15439,7 +15442,7 @@
       </c>
       <c r="B69" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3083</v>
+        <v>3057</v>
       </c>
       <c r="C69" s="1">
         <v>1068</v>
@@ -15457,7 +15460,7 @@
       </c>
       <c r="B70" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3091</v>
+        <v>3048</v>
       </c>
       <c r="C70" s="1">
         <v>1069</v>
@@ -15475,7 +15478,7 @@
       </c>
       <c r="B71" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3078</v>
+        <v>3024</v>
       </c>
       <c r="C71" s="1">
         <v>1070</v>
@@ -15493,7 +15496,7 @@
       </c>
       <c r="B72" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3087</v>
+        <v>3042</v>
       </c>
       <c r="C72" s="1">
         <v>1071</v>
@@ -15511,7 +15514,7 @@
       </c>
       <c r="B73" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3097</v>
+        <v>3090</v>
       </c>
       <c r="C73" s="1">
         <v>1072</v>
@@ -15529,7 +15532,7 @@
       </c>
       <c r="B74" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3065</v>
+        <v>3081</v>
       </c>
       <c r="C74" s="1">
         <v>1073</v>
@@ -15547,7 +15550,7 @@
       </c>
       <c r="B75" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3015</v>
+        <v>3074</v>
       </c>
       <c r="C75" s="1">
         <v>1074</v>
@@ -15565,7 +15568,7 @@
       </c>
       <c r="B76" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3009</v>
+        <v>3058</v>
       </c>
       <c r="C76" s="1">
         <v>1075</v>
@@ -15583,7 +15586,7 @@
       </c>
       <c r="B77" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3008</v>
+        <v>3022</v>
       </c>
       <c r="C77" s="1">
         <v>1076</v>
@@ -15601,7 +15604,7 @@
       </c>
       <c r="B78" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3080</v>
+        <v>3044</v>
       </c>
       <c r="C78" s="1">
         <v>1077</v>
@@ -15619,7 +15622,7 @@
       </c>
       <c r="B79" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3056</v>
+        <v>3041</v>
       </c>
       <c r="C79" s="1">
         <v>1078</v>
@@ -15637,7 +15640,7 @@
       </c>
       <c r="B80" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3078</v>
+        <v>3021</v>
       </c>
       <c r="C80" s="1">
         <v>1079</v>
@@ -15655,7 +15658,7 @@
       </c>
       <c r="B81" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3072</v>
+        <v>3055</v>
       </c>
       <c r="C81" s="1">
         <v>1080</v>
@@ -15673,7 +15676,7 @@
       </c>
       <c r="B82" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3056</v>
+        <v>3003</v>
       </c>
       <c r="C82" s="1">
         <v>1081</v>
@@ -15691,7 +15694,7 @@
       </c>
       <c r="B83" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3090</v>
+        <v>3059</v>
       </c>
       <c r="C83" s="1">
         <v>1082</v>
@@ -15709,7 +15712,7 @@
       </c>
       <c r="B84" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3087</v>
+        <v>3056</v>
       </c>
       <c r="C84" s="1">
         <v>1083</v>
@@ -15727,7 +15730,7 @@
       </c>
       <c r="B85" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3091</v>
+        <v>3038</v>
       </c>
       <c r="C85" s="1">
         <v>1084</v>
@@ -15745,7 +15748,7 @@
       </c>
       <c r="B86" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3029</v>
+        <v>3043</v>
       </c>
       <c r="C86" s="1">
         <v>1085</v>
@@ -15763,7 +15766,7 @@
       </c>
       <c r="B87" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3099</v>
+        <v>3064</v>
       </c>
       <c r="C87" s="1">
         <v>1086</v>
@@ -15799,7 +15802,7 @@
       </c>
       <c r="B89" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3051</v>
+        <v>3012</v>
       </c>
       <c r="C89" s="1">
         <v>1088</v>
@@ -15817,7 +15820,7 @@
       </c>
       <c r="B90" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3006</v>
+        <v>3002</v>
       </c>
       <c r="C90" s="1">
         <v>1089</v>
@@ -15835,7 +15838,7 @@
       </c>
       <c r="B91" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3093</v>
+        <v>3020</v>
       </c>
       <c r="C91" s="1">
         <v>1090</v>
@@ -15853,7 +15856,7 @@
       </c>
       <c r="B92" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3043</v>
+        <v>3036</v>
       </c>
       <c r="C92" s="1">
         <v>1091</v>
@@ -15871,7 +15874,7 @@
       </c>
       <c r="B93" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3002</v>
+        <v>3076</v>
       </c>
       <c r="C93" s="1">
         <v>1092</v>
@@ -15889,7 +15892,7 @@
       </c>
       <c r="B94" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3072</v>
+        <v>3049</v>
       </c>
       <c r="C94" s="1">
         <v>1093</v>
@@ -15907,7 +15910,7 @@
       </c>
       <c r="B95" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3060</v>
+        <v>3040</v>
       </c>
       <c r="C95" s="1">
         <v>1094</v>
@@ -15925,7 +15928,7 @@
       </c>
       <c r="B96" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3086</v>
+        <v>3019</v>
       </c>
       <c r="C96" s="1">
         <v>1095</v>
@@ -15943,7 +15946,7 @@
       </c>
       <c r="B97" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3031</v>
+        <v>3068</v>
       </c>
       <c r="C97" s="1">
         <v>1096</v>
@@ -15961,7 +15964,7 @@
       </c>
       <c r="B98" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3083</v>
+        <v>3034</v>
       </c>
       <c r="C98" s="1">
         <v>1097</v>
@@ -15979,7 +15982,7 @@
       </c>
       <c r="B99" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3001</v>
+        <v>3042</v>
       </c>
       <c r="C99" s="1">
         <v>1098</v>
@@ -15997,7 +16000,7 @@
       </c>
       <c r="B100" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3010</v>
+        <v>3043</v>
       </c>
       <c r="C100" s="1">
         <v>1099</v>
@@ -16015,7 +16018,7 @@
       </c>
       <c r="B101" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3024</v>
+        <v>3015</v>
       </c>
       <c r="C101" s="1">
         <v>1100</v>
@@ -16033,7 +16036,7 @@
       </c>
       <c r="B102" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3062</v>
+        <v>3043</v>
       </c>
       <c r="C102" s="1">
         <v>1101</v>
@@ -16051,7 +16054,7 @@
       </c>
       <c r="B103" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3020</v>
+        <v>3048</v>
       </c>
       <c r="C103" s="1">
         <v>1102</v>
@@ -16069,7 +16072,7 @@
       </c>
       <c r="B104" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3092</v>
+        <v>3090</v>
       </c>
       <c r="C104" s="1">
         <v>1103</v>
@@ -16087,7 +16090,7 @@
       </c>
       <c r="B105" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3019</v>
+        <v>3100</v>
       </c>
       <c r="C105" s="1">
         <v>1104</v>
@@ -16105,7 +16108,7 @@
       </c>
       <c r="B106" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3019</v>
+        <v>3090</v>
       </c>
       <c r="C106" s="1">
         <v>1105</v>
@@ -16123,7 +16126,7 @@
       </c>
       <c r="B107" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3098</v>
+        <v>3013</v>
       </c>
       <c r="C107" s="1">
         <v>1106</v>
@@ -16141,7 +16144,7 @@
       </c>
       <c r="B108" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3096</v>
+        <v>3026</v>
       </c>
       <c r="C108" s="1">
         <v>1107</v>
@@ -16159,7 +16162,7 @@
       </c>
       <c r="B109" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3081</v>
+        <v>3092</v>
       </c>
       <c r="C109" s="1">
         <v>1108</v>
@@ -16177,7 +16180,7 @@
       </c>
       <c r="B110" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3055</v>
+        <v>3073</v>
       </c>
       <c r="C110" s="1">
         <v>1109</v>

</xml_diff>